<commit_message>
Limit population data to what we actually need #2340
This allow us to "save" 41'580 records
</commit_message>
<xml_diff>
--- a/tests/data/import_population.xlsx
+++ b/tests/data/import_population.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="469" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="466" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>Major area, region, country or area</t>
   </si>
@@ -26,24 +26,6 @@
   </si>
   <si>
     <t>ISO-3</t>
-  </si>
-  <si>
-    <t>1950</t>
-  </si>
-  <si>
-    <t>1951</t>
-  </si>
-  <si>
-    <t>1952</t>
-  </si>
-  <si>
-    <t>1953</t>
-  </si>
-  <si>
-    <t>1954</t>
-  </si>
-  <si>
-    <t>1955</t>
   </si>
   <si>
     <t>Afghanistan</t>
@@ -72,7 +54,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -113,21 +95,21 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFC0C0C0"/>
       </left>
@@ -144,85 +126,85 @@
     </border>
   </borders>
   <cellStyleXfs count="22">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="20">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="20">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="20">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="21">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="21">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="21">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="21">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Normal_Feuil1" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Normal_Urban" xfId="21"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Feuil1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal_Urban" xfId="21" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -230,12 +212,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -247,7 +230,7 @@
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -257,34 +240,34 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1" t="n">
+        <v>1979</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>1980</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>1981</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>7450.738</v>
@@ -305,15 +288,15 @@
         <v>8009.614</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>1214.489</v>
@@ -334,15 +317,15 @@
         <v>1390.137</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>8872.247</v>
@@ -366,7 +349,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -377,12 +360,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -394,9 +378,9 @@
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -404,34 +388,34 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="n">
+        <v>1979</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>1980</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>1981</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="2">
-      <c r="A2" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="8" t="n">
         <v>432.143</v>
@@ -452,15 +436,15 @@
         <v>545.855</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3" s="8" t="n">
         <v>249.31</v>
@@ -481,15 +465,15 @@
         <v>373.446</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" s="8" t="n">
         <v>1970.792</v>
@@ -513,7 +497,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -524,12 +508,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -541,9 +526,9 @@
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -551,34 +536,34 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="n">
+        <v>1979</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>1980</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>1981</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
-      <c r="A2" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">Total!D2-Urban!D2</f>
@@ -605,15 +590,15 @@
         <v>7463.759</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">Total!D3-Urban!D3</f>
@@ -640,15 +625,15 @@
         <v>1016.691</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">Total!D4-Urban!D4</f>
@@ -678,7 +663,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>